<commit_message>
permissions v-0.9:html tags "add"
</commit_message>
<xml_diff>
--- a/permissons.xlsx
+++ b/permissons.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20369"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FCAA774-C161-495F-BB8C-86D58BFFB1A8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D53050B3-099A-45FA-8EE4-7C04F4E7DEE5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="120">
   <si>
     <t>权限名</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -486,6 +486,18 @@
   </si>
   <si>
     <t>/memberLevel/editMember</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">        新增</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>add</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/addArchives</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -493,7 +505,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -517,6 +529,13 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -538,9 +557,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -821,10 +841,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -870,56 +890,56 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C4" t="s">
-        <v>92</v>
+    <row r="4" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B5" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C6" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
         <v>34</v>
@@ -927,76 +947,76 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>65</v>
+        <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>96</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C15" t="s">
         <v>97</v>
@@ -1004,331 +1024,342 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
       <c r="B17" t="s">
-        <v>4</v>
+        <v>68</v>
       </c>
       <c r="C17" t="s">
-        <v>11</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>69</v>
+        <v>4</v>
       </c>
       <c r="C18" t="s">
-        <v>99</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C19" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C20" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="B21" t="s">
-        <v>5</v>
+        <v>71</v>
       </c>
       <c r="C21" t="s">
-        <v>12</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>59</v>
+        <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>72</v>
+        <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>102</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B24" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C24" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="B25" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C25" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="B26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C26" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="B27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C27" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>76</v>
       </c>
       <c r="B28" t="s">
-        <v>6</v>
+        <v>79</v>
       </c>
       <c r="C28" t="s">
-        <v>13</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B29" t="s">
-        <v>80</v>
+        <v>6</v>
       </c>
       <c r="C29" t="s">
-        <v>108</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B30" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B31" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C31" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="B32" t="s">
-        <v>7</v>
+        <v>82</v>
       </c>
       <c r="C32" t="s">
-        <v>14</v>
+        <v>110</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>59</v>
+        <v>27</v>
       </c>
       <c r="B33" t="s">
-        <v>83</v>
+        <v>7</v>
       </c>
       <c r="C33" t="s">
-        <v>111</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B34" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C34" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B35" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C35" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="B36" t="s">
-        <v>47</v>
+        <v>85</v>
       </c>
       <c r="C36" t="s">
-        <v>19</v>
+        <v>113</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="B37" t="s">
-        <v>86</v>
+        <v>47</v>
       </c>
       <c r="C37" t="s">
-        <v>115</v>
+        <v>19</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B38" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C38" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B39" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C39" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="B40" t="s">
-        <v>20</v>
+        <v>88</v>
       </c>
       <c r="C40" t="s">
-        <v>39</v>
+        <v>114</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="B41" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="C41" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C42" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C43" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B44" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C44" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>45</v>
+      </c>
+      <c r="B45" t="s">
+        <v>51</v>
+      </c>
+      <c r="C45" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>89</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>90</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C46" t="s">
         <v>91</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed bug & update doc
</commit_message>
<xml_diff>
--- a/permissons.xlsx
+++ b/permissons.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20369"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D53050B3-099A-45FA-8EE4-7C04F4E7DEE5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B4236EB-89A7-4E3C-AD1E-1C59FE597526}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="121">
   <si>
     <t>权限名</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -34,26 +34,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>coupon:list</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>consumeType:list</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>consumeItem:list</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insuranceCompany:list</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insuranceType:list</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>根权限</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -62,50 +42,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/coupon/getCouponList</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/consumeType/getConsumeTypeList</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/consumeProject/getConsumeProjectNameList</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/insuranceCompany/getInsuranceCompanyList</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/insuranceType/getInsuranceTypeList</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/service</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>memberUseCoupon</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>customParameters</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/parameters</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/membershipLevel/getMemberList</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>statistics</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">    微会员用卡</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -154,42 +94,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>useCoupon</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/useCoupon</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cancelConsume</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/cancelConsume</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>review</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/review</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/statistics</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>useCoupon</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/useCouponHistory</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">        用卡历史</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -206,50 +110,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>rollback</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>memberLevel:list</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/cancelConsumeHistory</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>coupon</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/couponStatistical</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>balance</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/balanceStatistical</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">    微会员/会员档案</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>archives</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">        修改&amp;查看具体信息</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>more</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">        删除</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -274,54 +142,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>delete</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>level</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>coupon:add</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>coupon:edit</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>coupon:delete</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>coupon:relItem</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>consumeType:add</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>consumeType:edit</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>consumeType:delete</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>consumeItem:add</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>consumeItem:edit</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>consumeItem:delete</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">            关联消费卡券</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -330,174 +150,359 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>consumeItem:relCoupon</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>consumeItem:relItem</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>consumeItem:speItem</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insuranceCompany:add</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insuranceCompany:edit</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insuranceCompany:delete</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insuranceType:add</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insuranceType:edit</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insuranceType:delete</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>memberLevel:add</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>memberLevel:edit</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>memberLevel:delete</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">    系统管理</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>management</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/manage</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/more</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/level</t>
-  </si>
-  <si>
-    <t>/deleteArchives</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/archives</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/coupon/addCoupon</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/coupon/editCoupon</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/coupon/relateConsumeProject</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/consumeType/addConsumeType</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/consumeType/deleteConsumeType</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/consumeType/editConsumeType</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/consumeItem/addConsumeProject</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/consumeItem/editConsumeProject</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/consumeItem/relateCoupon</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/consumeItem/deleteConsumeProject</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/consumeItem/relateConsumeProject</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/consumeItem/practicalProject</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/insuranceCompany/addInsuranceCompany</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/insuranceCompany/editInsuranceCompany</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/insuranceCompany/deleteInsuranceCompany</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/insuranceType/addInsuranceType</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/insuranceType/editInsuranceType</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/insuranceType/deleteInsuranceType</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/memberLevel/deleteMember</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/memberLevel/addMember</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/memberLevel/editMember</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">        新增</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>add</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/addArchives</t>
+    <t>member:archives</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member:management</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member:statistics</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member:customParameters</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member:memberUseCoupon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member:archives:add</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member:archives:more</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member:archives:delete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member:archives:level</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member:memberUseCoupon:useCoupon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member:memberUseCoupon:cancelConsume</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member:memberUseCoupon:review</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member:customParameters:coupon:list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member:customParameters:coupon:add</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member:customParameters:coupon:edit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member:customParameters:coupon:delete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member:customParameters:coupon:relItem</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member:customParameters:consumeType:list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member:customParameters:consumeType:add</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member:customParameters:consumeType:edit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member:customParameters:consumeType:delete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member:customParameters:consumeItem:list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member:customParameters:consumeItem:add</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member:customParameters:consumeItem:edit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member:customParameters:consumeItem:delete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member:customParameters:consumeItem:relCoupon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member:customParameters:consumeItem:relItem</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member:customParameters:consumeItem:speItem</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member:customParameters:insuranceCompany:list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member:customParameters:insuranceCompany:add</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member:customParameters:insuranceCompany:edit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member:customParameters:insuranceCompany:delete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member:customParameters:insuranceType:list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member:customParameters:insuranceType:add</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member:customParameters:insuranceType:edit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member:customParameters:insuranceType:delete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member:customParameters:memberLevel:list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member:customParameters:memberLevel:add</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member:customParameters:memberLevel:edit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member:customParameters:memberLevel:delete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member:statistics:useCoupon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member:statistics:rollback</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member:statistics:coupon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>member:statistics:balance</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/service/archives</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/service/useCoupon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/service/parameters</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/service/manage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/service/statistics/useCouponHistory</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/service/statistics/cancelConsumeHistory</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/service/statistics/couponStatistical</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/service/statistics/balanceStatistical</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/service/statistics</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/service/archives/addArchives</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/service/archives/deleteArchives</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/service/archives/level</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/service/useCoupon/useCoupon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/service/useCoupon/cancelConsume</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/service/useCoupon/review</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/service/parameters/coupon/getCouponList</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/service/parameters/coupon/addCoupon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/service/parameters/coupon/editCoupon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/service/parameters/coupon/relateConsumeProject</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/service/parameters/consumeType/getConsumeTypeList</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/service/parameters/consumeType/addConsumeType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/service/parameters/consumeType/editConsumeType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/service/parameters/consumeType/deleteConsumeType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/service/parameters/consumeItem/addConsumeProject</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/service/parameters/consumeItem/editConsumeProject</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/service/parameters/consumeItem/deleteConsumeProject</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/service/parameters/consumeItem/relateCoupon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/service/parameters/consumeItem/relateConsumeProject</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/service/parameters/consumeItem/practicalProject</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/service/parameters/insuranceCompany/getInsuranceCompanyList</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/service/parameters/insuranceCompany/addInsuranceCompany</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/service/parameters/insuranceCompany/editInsuranceCompany</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/service/parameters/insuranceCompany/deleteInsuranceCompany</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/service/parameters/insuranceType/getInsuranceTypeList</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/service/parameters/insuranceType/addInsuranceType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/service/parameters/insuranceType/editInsuranceType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/service/parameters/insuranceType/deleteInsuranceType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/service/parameters/membershipLevel/getMemberList</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/service/archives/editArchives</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/service/parameters/consumeItem/getConsumeProjectList</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/service/parameters/membershipLevel/addMember</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/service/parameters/membershipLevel/editMember</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/service/parameters/membershipLevel/deleteMember</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -844,7 +849,7 @@
   <dimension ref="A1:C46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -870,219 +875,219 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>117</v>
+        <v>33</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>118</v>
+        <v>39</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>119</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>92</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>3</v>
+        <v>46</v>
       </c>
       <c r="C13" t="s">
-        <v>10</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="C14" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="C15" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>62</v>
+        <v>29</v>
       </c>
       <c r="B16" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="C16" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>61</v>
+        <v>28</v>
       </c>
       <c r="B17" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="C17" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="C18" t="s">
-        <v>11</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B19" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="C19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="C20" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>62</v>
+        <v>29</v>
       </c>
       <c r="B21" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="C21" t="s">
         <v>100</v>
@@ -1090,54 +1095,54 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="B22" t="s">
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="C22" t="s">
-        <v>12</v>
+        <v>117</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B23" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="C24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>62</v>
+        <v>29</v>
       </c>
       <c r="B25" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="C25" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>75</v>
+        <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="C26" t="s">
         <v>104</v>
@@ -1145,43 +1150,43 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>61</v>
+        <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="C27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B28" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="C28" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="B29" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="C29" t="s">
-        <v>13</v>
+        <v>107</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B30" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="C30" t="s">
         <v>108</v>
@@ -1189,10 +1194,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B31" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="C31" t="s">
         <v>109</v>
@@ -1200,10 +1205,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>62</v>
+        <v>29</v>
       </c>
       <c r="B32" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="C32" t="s">
         <v>110</v>
@@ -1211,156 +1216,156 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="B33" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
       <c r="C33" t="s">
-        <v>14</v>
+        <v>111</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B34" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="C34" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B35" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="C35" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>62</v>
+        <v>29</v>
       </c>
       <c r="B36" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="C36" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B37" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="C37" t="s">
-        <v>19</v>
+        <v>115</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B38" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="C38" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B39" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="C39" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>62</v>
+        <v>29</v>
       </c>
       <c r="B40" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="C40" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="B41" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="C41" t="s">
-        <v>39</v>
+        <v>86</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="B42" t="s">
-        <v>40</v>
+        <v>74</v>
       </c>
       <c r="C42" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="B43" t="s">
-        <v>46</v>
+        <v>75</v>
       </c>
       <c r="C43" t="s">
-        <v>48</v>
+        <v>83</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="B44" t="s">
-        <v>49</v>
+        <v>76</v>
       </c>
       <c r="C44" t="s">
-        <v>50</v>
+        <v>84</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="B45" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="C45" t="s">
-        <v>52</v>
+        <v>85</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>89</v>
+        <v>32</v>
       </c>
       <c r="B46" t="s">
-        <v>90</v>
+        <v>35</v>
       </c>
       <c r="C46" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
separate the manage permission
</commit_message>
<xml_diff>
--- a/permissons.xlsx
+++ b/permissons.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20369"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B4236EB-89A7-4E3C-AD1E-1C59FE597526}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17888833-416C-446C-81F8-9B5EFACC4307}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="122">
   <si>
     <t>权限名</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -503,6 +503,10 @@
   </si>
   <si>
     <t>/service/parameters/membershipLevel/deleteMember</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/service/parameters/coupon/deleteCoupon</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -849,7 +853,7 @@
   <dimension ref="A1:C46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1035,7 +1039,7 @@
         <v>49</v>
       </c>
       <c r="C16" t="s">
-        <v>95</v>
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>